<commit_message>
Update templates's versions for testing purposes
</commit_message>
<xml_diff>
--- a/templates/1SPL01_plants.xlsx
+++ b/templates/1SPL01_plants.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\omaus\SWATE_templates\templates\1SPL01_plants\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\omaus\SWATE_templates\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85DAC0D6-0303-46B7-B9E1-BAD4CB496697}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65EF0BAF-65B1-46B6-A826-19E531F88CCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{2D1671A6-E5E6-4E90-817E-C23847CD9BD1}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2D1671A6-E5E6-4E90-817E-C23847CD9BD1}"/>
   </bookViews>
   <sheets>
     <sheet name="1SPL01_plants" sheetId="1" r:id="rId1"/>
@@ -46,11 +46,11 @@
   <commentList>
     <comment ref="A1" authorId="0" shapeId="0" xr:uid="{A6730C41-F5DE-4F01-A3FC-095AF4373E4D}">
       <text>
-        <t>[Kommentarthread]
-Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
-Kommentar:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     The unique identifier of this template. It will be auto generated.
-Antwort:
+Reply:
     id=f12e98ee-a4e7-4ada-ba56-1e13cce1a44b</t>
       </text>
     </comment>
@@ -1237,7 +1237,7 @@
     <t>http://purl.obolibrary.org/obo/UO_0000027</t>
   </si>
   <si>
-    <t>1.1.9</t>
+    <t>1.1.10</t>
   </si>
 </sst>
 </file>
@@ -1447,8 +1447,8 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 3" xfId="1" xr:uid="{D09CA6D9-E6C7-4433-8F48-8CA6F5BF0770}"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="53">
     <dxf>
@@ -1762,7 +1762,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2102,9 +2102,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F8916BF-D1BA-4E62-B448-EB2F6971FAFB}">
   <dimension ref="A1:DN7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29.42578125" bestFit="1" customWidth="1"/>
@@ -3371,9 +3371,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C806736B-09AD-44FE-B8F6-60FEE51F74DE}">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="57.140625" customWidth="1"/>
@@ -3641,7 +3641,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="44.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
@@ -5156,7 +5156,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="44.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
@@ -6703,7 +6703,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="44.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
@@ -8122,7 +8122,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="44.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
test edit template metadata
</commit_message>
<xml_diff>
--- a/templates/1SPL01_plants.xlsx
+++ b/templates/1SPL01_plants.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20340"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\git\templates\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dominikbrilhaus/03_DataPLANT_github/SWATE_templates/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DF622A41-14C2-427F-97AF-3F5E6D052462}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EE78103-3C6E-1742-8A3E-115735EF6AA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="3" xr2:uid="{2D1671A6-E5E6-4E90-817E-C23847CD9BD1}"/>
+    <workbookView xWindow="360" yWindow="-20260" windowWidth="25500" windowHeight="16120" activeTab="1" xr2:uid="{2D1671A6-E5E6-4E90-817E-C23847CD9BD1}"/>
   </bookViews>
   <sheets>
     <sheet name="1SPL01_plants" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2431" uniqueCount="452">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2433" uniqueCount="454">
   <si>
     <t>Source Name</t>
   </si>
@@ -1425,6 +1425,12 @@
   </si>
   <si>
     <t>https://www.ebi.ac.uk/ena/browser/view/ERC000037 https://www.ebi.ac.uk/ena/browser/view/ERC000020</t>
+  </si>
+  <si>
+    <t>[Comment] ER checklist source</t>
+  </si>
+  <si>
+    <t>[Comment] Author ORCID</t>
   </si>
 </sst>
 </file>
@@ -1599,7 +1605,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1645,6 +1651,9 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2439,7 +2448,7 @@
       <selection activeCell="DX1" sqref="DX1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30" bestFit="1" customWidth="1"/>
@@ -2457,22 +2466,22 @@
     <col min="14" max="14" width="25.6640625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="36.6640625" hidden="1" customWidth="1"/>
     <col min="16" max="16" width="43.6640625" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="25.88671875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="25.83203125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="36.6640625" hidden="1" customWidth="1"/>
     <col min="19" max="19" width="43.6640625" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="27.5546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="27.5" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="36.6640625" hidden="1" customWidth="1"/>
     <col min="22" max="22" width="43.6640625" hidden="1" customWidth="1"/>
     <col min="23" max="23" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="30.88671875" hidden="1" customWidth="1"/>
-    <col min="25" max="25" width="37.88671875" hidden="1" customWidth="1"/>
+    <col min="24" max="24" width="30.83203125" hidden="1" customWidth="1"/>
+    <col min="25" max="25" width="37.83203125" hidden="1" customWidth="1"/>
     <col min="26" max="26" width="31.6640625" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="36.6640625" hidden="1" customWidth="1"/>
     <col min="28" max="28" width="43.6640625" hidden="1" customWidth="1"/>
-    <col min="29" max="29" width="25.88671875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="25.83203125" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="36.6640625" hidden="1" customWidth="1"/>
     <col min="31" max="31" width="43.6640625" hidden="1" customWidth="1"/>
-    <col min="32" max="32" width="26.5546875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="26.5" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="36.6640625" hidden="1" customWidth="1"/>
     <col min="34" max="34" width="43.6640625" hidden="1" customWidth="1"/>
     <col min="35" max="35" width="30.33203125" bestFit="1" customWidth="1"/>
@@ -2481,43 +2490,43 @@
     <col min="38" max="38" width="38.33203125" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="36.6640625" hidden="1" customWidth="1"/>
     <col min="40" max="40" width="43.6640625" hidden="1" customWidth="1"/>
-    <col min="41" max="41" width="30.5546875" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="30.5" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="36.6640625" hidden="1" customWidth="1"/>
     <col min="43" max="43" width="43.6640625" hidden="1" customWidth="1"/>
     <col min="44" max="44" width="36" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="36.6640625" hidden="1" customWidth="1"/>
     <col min="46" max="46" width="43.6640625" hidden="1" customWidth="1"/>
-    <col min="47" max="47" width="28.5546875" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="28.5" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="36.6640625" hidden="1" customWidth="1"/>
     <col min="49" max="49" width="43.6640625" hidden="1" customWidth="1"/>
-    <col min="50" max="50" width="33.44140625" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="30.109375" hidden="1" customWidth="1"/>
-    <col min="52" max="52" width="37.109375" hidden="1" customWidth="1"/>
+    <col min="50" max="50" width="33.5" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="30.1640625" hidden="1" customWidth="1"/>
+    <col min="52" max="52" width="37.1640625" hidden="1" customWidth="1"/>
     <col min="53" max="53" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="32.44140625" hidden="1" customWidth="1"/>
-    <col min="55" max="55" width="39.5546875" hidden="1" customWidth="1"/>
-    <col min="56" max="56" width="47.5546875" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="32.44140625" hidden="1" customWidth="1"/>
-    <col min="58" max="58" width="39.5546875" hidden="1" customWidth="1"/>
-    <col min="59" max="59" width="35.88671875" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="32.5" hidden="1" customWidth="1"/>
+    <col min="55" max="55" width="39.5" hidden="1" customWidth="1"/>
+    <col min="56" max="56" width="47.5" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="32.5" hidden="1" customWidth="1"/>
+    <col min="58" max="58" width="39.5" hidden="1" customWidth="1"/>
+    <col min="59" max="59" width="35.83203125" bestFit="1" customWidth="1"/>
     <col min="60" max="60" width="36.6640625" hidden="1" customWidth="1"/>
     <col min="61" max="61" width="43.6640625" hidden="1" customWidth="1"/>
     <col min="62" max="62" width="35.6640625" bestFit="1" customWidth="1"/>
     <col min="63" max="63" width="36.6640625" hidden="1" customWidth="1"/>
     <col min="64" max="64" width="43.6640625" hidden="1" customWidth="1"/>
-    <col min="65" max="65" width="40.109375" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="7.109375" hidden="1" customWidth="1"/>
-    <col min="67" max="67" width="32.44140625" hidden="1" customWidth="1"/>
-    <col min="68" max="68" width="39.5546875" hidden="1" customWidth="1"/>
+    <col min="65" max="65" width="40.1640625" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="7.1640625" hidden="1" customWidth="1"/>
+    <col min="67" max="67" width="32.5" hidden="1" customWidth="1"/>
+    <col min="68" max="68" width="39.5" hidden="1" customWidth="1"/>
     <col min="69" max="69" width="31" bestFit="1" customWidth="1"/>
     <col min="70" max="70" width="11" hidden="1" customWidth="1"/>
     <col min="71" max="71" width="36.6640625" hidden="1" customWidth="1"/>
     <col min="72" max="72" width="43.6640625" hidden="1" customWidth="1"/>
-    <col min="73" max="73" width="32.5546875" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="32.5" bestFit="1" customWidth="1"/>
     <col min="74" max="74" width="11" hidden="1" customWidth="1"/>
     <col min="75" max="75" width="36.6640625" hidden="1" customWidth="1"/>
     <col min="76" max="76" width="43.6640625" hidden="1" customWidth="1"/>
-    <col min="77" max="77" width="34.5546875" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="34.5" bestFit="1" customWidth="1"/>
     <col min="78" max="78" width="11" hidden="1" customWidth="1"/>
     <col min="79" max="79" width="36.6640625" hidden="1" customWidth="1"/>
     <col min="80" max="80" width="43.6640625" hidden="1" customWidth="1"/>
@@ -2526,30 +2535,30 @@
     <col min="83" max="83" width="36.6640625" hidden="1" customWidth="1"/>
     <col min="84" max="84" width="43.6640625" hidden="1" customWidth="1"/>
     <col min="85" max="85" width="35.6640625" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="32.44140625" hidden="1" customWidth="1"/>
-    <col min="87" max="87" width="39.5546875" hidden="1" customWidth="1"/>
-    <col min="88" max="88" width="40.44140625" bestFit="1" customWidth="1"/>
-    <col min="89" max="89" width="32.44140625" hidden="1" customWidth="1"/>
-    <col min="90" max="90" width="39.5546875" hidden="1" customWidth="1"/>
+    <col min="86" max="86" width="32.5" hidden="1" customWidth="1"/>
+    <col min="87" max="87" width="39.5" hidden="1" customWidth="1"/>
+    <col min="88" max="88" width="40.5" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="32.5" hidden="1" customWidth="1"/>
+    <col min="90" max="90" width="39.5" hidden="1" customWidth="1"/>
     <col min="91" max="91" width="39" bestFit="1" customWidth="1"/>
-    <col min="92" max="92" width="32.44140625" hidden="1" customWidth="1"/>
-    <col min="93" max="93" width="39.5546875" hidden="1" customWidth="1"/>
+    <col min="92" max="92" width="32.5" hidden="1" customWidth="1"/>
+    <col min="93" max="93" width="39.5" hidden="1" customWidth="1"/>
     <col min="94" max="94" width="38" bestFit="1" customWidth="1"/>
-    <col min="95" max="95" width="32.44140625" hidden="1" customWidth="1"/>
-    <col min="96" max="96" width="39.5546875" hidden="1" customWidth="1"/>
-    <col min="97" max="97" width="33.88671875" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="32.5" hidden="1" customWidth="1"/>
+    <col min="96" max="96" width="39.5" hidden="1" customWidth="1"/>
+    <col min="97" max="97" width="33.83203125" bestFit="1" customWidth="1"/>
     <col min="98" max="98" width="36.6640625" hidden="1" customWidth="1"/>
     <col min="99" max="99" width="43.6640625" hidden="1" customWidth="1"/>
-    <col min="100" max="100" width="39.88671875" bestFit="1" customWidth="1"/>
+    <col min="100" max="100" width="39.83203125" bestFit="1" customWidth="1"/>
     <col min="101" max="101" width="36.6640625" hidden="1" customWidth="1"/>
     <col min="102" max="102" width="43.6640625" hidden="1" customWidth="1"/>
     <col min="103" max="103" width="37.33203125" bestFit="1" customWidth="1"/>
     <col min="104" max="104" width="36.6640625" hidden="1" customWidth="1"/>
     <col min="105" max="105" width="43.6640625" hidden="1" customWidth="1"/>
-    <col min="106" max="106" width="28.5546875" bestFit="1" customWidth="1"/>
+    <col min="106" max="106" width="28.5" bestFit="1" customWidth="1"/>
     <col min="107" max="107" width="36.6640625" hidden="1" customWidth="1"/>
     <col min="108" max="108" width="43.6640625" hidden="1" customWidth="1"/>
-    <col min="109" max="109" width="39.109375" bestFit="1" customWidth="1"/>
+    <col min="109" max="109" width="39.1640625" bestFit="1" customWidth="1"/>
     <col min="110" max="110" width="36.6640625" hidden="1" customWidth="1"/>
     <col min="111" max="111" width="43.6640625" hidden="1" customWidth="1"/>
     <col min="112" max="112" width="43.6640625" bestFit="1" customWidth="1"/>
@@ -2558,40 +2567,40 @@
     <col min="115" max="115" width="29" bestFit="1" customWidth="1"/>
     <col min="116" max="116" width="36.6640625" hidden="1" customWidth="1"/>
     <col min="117" max="117" width="43.6640625" hidden="1" customWidth="1"/>
-    <col min="118" max="118" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="118" max="118" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="119" max="119" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="120" max="120" width="38.109375" hidden="1" customWidth="1"/>
-    <col min="121" max="121" width="45.109375" hidden="1" customWidth="1"/>
+    <col min="120" max="120" width="38.1640625" hidden="1" customWidth="1"/>
+    <col min="121" max="121" width="45.1640625" hidden="1" customWidth="1"/>
     <col min="122" max="122" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="123" max="123" width="38.109375" hidden="1" customWidth="1"/>
-    <col min="124" max="124" width="45.109375" hidden="1" customWidth="1"/>
+    <col min="123" max="123" width="38.1640625" hidden="1" customWidth="1"/>
+    <col min="124" max="124" width="45.1640625" hidden="1" customWidth="1"/>
     <col min="125" max="125" width="32.33203125" bestFit="1" customWidth="1"/>
-    <col min="126" max="126" width="31.5546875" hidden="1" customWidth="1"/>
-    <col min="127" max="127" width="38.5546875" hidden="1" customWidth="1"/>
+    <col min="126" max="126" width="31.5" hidden="1" customWidth="1"/>
+    <col min="127" max="127" width="38.5" hidden="1" customWidth="1"/>
     <col min="128" max="128" width="27" bestFit="1" customWidth="1"/>
-    <col min="129" max="129" width="38.109375" hidden="1" customWidth="1"/>
-    <col min="130" max="130" width="45.109375" hidden="1" customWidth="1"/>
+    <col min="129" max="129" width="38.1640625" hidden="1" customWidth="1"/>
+    <col min="130" max="130" width="45.1640625" hidden="1" customWidth="1"/>
     <col min="131" max="131" width="33" bestFit="1" customWidth="1"/>
-    <col min="132" max="132" width="38.109375" hidden="1" customWidth="1"/>
-    <col min="133" max="133" width="45.109375" hidden="1" customWidth="1"/>
+    <col min="132" max="132" width="38.1640625" hidden="1" customWidth="1"/>
+    <col min="133" max="133" width="45.1640625" hidden="1" customWidth="1"/>
     <col min="134" max="134" width="31.33203125" bestFit="1" customWidth="1"/>
-    <col min="135" max="135" width="38.109375" hidden="1" customWidth="1"/>
-    <col min="136" max="136" width="45.109375" hidden="1" customWidth="1"/>
-    <col min="137" max="137" width="39.109375" bestFit="1" customWidth="1"/>
-    <col min="138" max="138" width="38.109375" hidden="1" customWidth="1"/>
-    <col min="139" max="139" width="45.109375" hidden="1" customWidth="1"/>
-    <col min="140" max="140" width="55.88671875" bestFit="1" customWidth="1"/>
-    <col min="141" max="141" width="38.109375" hidden="1" customWidth="1"/>
-    <col min="142" max="142" width="45.109375" hidden="1" customWidth="1"/>
-    <col min="143" max="143" width="24.44140625" bestFit="1" customWidth="1"/>
+    <col min="135" max="135" width="38.1640625" hidden="1" customWidth="1"/>
+    <col min="136" max="136" width="45.1640625" hidden="1" customWidth="1"/>
+    <col min="137" max="137" width="39.1640625" bestFit="1" customWidth="1"/>
+    <col min="138" max="138" width="38.1640625" hidden="1" customWidth="1"/>
+    <col min="139" max="139" width="45.1640625" hidden="1" customWidth="1"/>
+    <col min="140" max="140" width="55.83203125" bestFit="1" customWidth="1"/>
+    <col min="141" max="141" width="38.1640625" hidden="1" customWidth="1"/>
+    <col min="142" max="142" width="45.1640625" hidden="1" customWidth="1"/>
+    <col min="143" max="143" width="24.5" bestFit="1" customWidth="1"/>
     <col min="144" max="144" width="35.33203125" hidden="1" customWidth="1"/>
     <col min="145" max="145" width="42.33203125" hidden="1" customWidth="1"/>
     <col min="146" max="146" width="40" bestFit="1" customWidth="1"/>
-    <col min="147" max="147" width="38.109375" hidden="1" customWidth="1"/>
-    <col min="148" max="148" width="45.109375" hidden="1" customWidth="1"/>
+    <col min="147" max="147" width="38.1640625" hidden="1" customWidth="1"/>
+    <col min="148" max="148" width="45.1640625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:148" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:148" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3037,7 +3046,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="2" spans="1:148" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:148" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>148</v>
       </c>
@@ -3251,7 +3260,7 @@
       <c r="EQ2" s="3"/>
       <c r="ER2" s="3"/>
     </row>
-    <row r="3" spans="1:148" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:148" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>173</v>
       </c>
@@ -3444,7 +3453,7 @@
       <c r="EQ3" s="3"/>
       <c r="ER3" s="3"/>
     </row>
-    <row r="4" spans="1:148" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:148" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>184</v>
       </c>
@@ -3613,7 +3622,7 @@
       <c r="EQ4" s="3"/>
       <c r="ER4" s="3"/>
     </row>
-    <row r="5" spans="1:148" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:148" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>193</v>
       </c>
@@ -3746,7 +3755,7 @@
       <c r="EQ5" s="3"/>
       <c r="ER5" s="3"/>
     </row>
-    <row r="6" spans="1:148" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:148" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>195</v>
       </c>
@@ -3870,7 +3879,7 @@
       <c r="EQ6" s="3"/>
       <c r="ER6" s="3"/>
     </row>
-    <row r="7" spans="1:148" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:148" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>196</v>
       </c>
@@ -4004,22 +4013,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C806736B-09AD-44FE-B8F6-60FEE51F74DE}">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="106" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="35.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="57.109375" customWidth="1"/>
-    <col min="3" max="3" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.1640625" customWidth="1"/>
+    <col min="3" max="3" width="14.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="57.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>197</v>
       </c>
@@ -4027,7 +4037,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>199</v>
       </c>
@@ -4035,7 +4045,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>201</v>
       </c>
@@ -4043,7 +4053,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>202</v>
       </c>
@@ -4051,19 +4061,19 @@
         <v>203</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>204</v>
       </c>
       <c r="B5" s="9"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>205</v>
       </c>
       <c r="B6" s="9"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>206</v>
       </c>
@@ -4071,13 +4081,13 @@
         <v>207</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>208</v>
       </c>
       <c r="B8" s="10"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>209</v>
       </c>
@@ -4097,7 +4107,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>215</v>
       </c>
@@ -4107,7 +4117,7 @@
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>216</v>
       </c>
@@ -4117,187 +4127,206 @@
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
+        <v>452</v>
+      </c>
+      <c r="B12" s="9"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="9"/>
+    </row>
+    <row r="13" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="B12" s="10"/>
-      <c r="F12" s="9"/>
-    </row>
-    <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
+      <c r="B13" s="10"/>
+      <c r="F13" s="9"/>
+    </row>
+    <row r="14" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B14" s="11" t="s">
         <v>219</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C14" s="9" t="s">
         <v>220</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D14" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="E14" s="9" t="s">
         <v>221</v>
       </c>
-      <c r="F13" s="9" t="s">
+      <c r="F14" s="9" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
         <v>223</v>
-      </c>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-    </row>
-    <row r="15" spans="1:6" ht="144" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="s">
-        <v>224</v>
       </c>
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
       <c r="E15" s="9"/>
-      <c r="F15" s="18" t="s">
+      <c r="F15" s="9"/>
+    </row>
+    <row r="16" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="18" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="6" t="s">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="6" t="s">
         <v>225</v>
       </c>
-      <c r="B16" s="10"/>
-      <c r="F16" s="9"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="5" t="s">
+      <c r="B17" s="10"/>
+      <c r="F17" s="9"/>
+    </row>
+    <row r="18" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" s="5" t="s">
         <v>226</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B18" s="11" t="s">
         <v>227</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C18" s="9" t="s">
         <v>228</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="D18" s="9" t="s">
         <v>229</v>
       </c>
-      <c r="F17" s="9" t="s">
+      <c r="F18" s="9" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="5" t="s">
+    <row r="19" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
         <v>231</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B19" s="9" t="s">
         <v>232</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C19" s="9" t="s">
         <v>233</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="D19" s="9" t="s">
         <v>234</v>
       </c>
-      <c r="F18" s="9" t="s">
+      <c r="F19" s="9" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="5" t="s">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
         <v>236</v>
-      </c>
-      <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="F19" s="9"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="5" t="s">
-        <v>237</v>
       </c>
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
       <c r="F20" s="9"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
       <c r="F21" s="9"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
       <c r="D22" s="9"/>
       <c r="F22" s="9"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
       <c r="F23" s="9"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
       <c r="F24" s="9"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="6" t="s">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="F25" s="9"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="5" t="s">
+        <v>453</v>
+      </c>
+      <c r="B26" s="9"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="19"/>
+      <c r="F26" s="9"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="6" t="s">
         <v>242</v>
       </c>
-      <c r="B25" s="10"/>
-      <c r="F25" s="9"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="5" t="s">
+      <c r="B27" s="10"/>
+      <c r="F27" s="9"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="5" t="s">
         <v>243</v>
       </c>
-      <c r="B26" s="11"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="9"/>
-      <c r="F26" s="9"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="5" t="s">
-        <v>244</v>
-      </c>
-      <c r="B27" s="9"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="9"/>
-      <c r="F27" s="9"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="7" t="s">
-        <v>245</v>
-      </c>
-      <c r="B28" s="12"/>
+      <c r="B28" s="11"/>
       <c r="C28" s="9"/>
       <c r="D28" s="9"/>
       <c r="F28" s="9"/>
     </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="F29" s="9"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="B30" s="12"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="F30" s="9"/>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F15" r:id="rId1" display="https://www.ebi.ac.uk/ena/browser/view/ERC000037" xr:uid="{8661B25F-28B7-4001-B986-A010D408E879}"/>
+    <hyperlink ref="F16" r:id="rId1" display="https://www.ebi.ac.uk/ena/browser/view/ERC000037" xr:uid="{8661B25F-28B7-4001-B986-A010D408E879}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -4311,23 +4340,23 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="44.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="46.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="30.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5546875" customWidth="1"/>
-    <col min="9" max="9" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5" customWidth="1"/>
+    <col min="9" max="9" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
         <v>246</v>
       </c>
@@ -4365,7 +4394,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
         <v>0</v>
       </c>
@@ -4401,7 +4430,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
         <v>117</v>
       </c>
@@ -4437,7 +4466,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
         <v>1</v>
       </c>
@@ -4475,7 +4504,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>4</v>
       </c>
@@ -4513,7 +4542,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
         <v>7</v>
       </c>
@@ -4549,7 +4578,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
         <v>10</v>
       </c>
@@ -4587,7 +4616,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
         <v>13</v>
       </c>
@@ -4625,7 +4654,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
         <v>16</v>
       </c>
@@ -4663,7 +4692,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
         <v>19</v>
       </c>
@@ -4701,7 +4730,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
         <v>22</v>
       </c>
@@ -4739,7 +4768,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
         <v>25</v>
       </c>
@@ -4777,7 +4806,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="14" t="s">
         <v>28</v>
       </c>
@@ -4815,7 +4844,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="14" t="s">
         <v>31</v>
       </c>
@@ -4853,7 +4882,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>294</v>
       </c>
@@ -4891,7 +4920,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="14" t="s">
         <v>37</v>
       </c>
@@ -4929,7 +4958,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="14" t="s">
         <v>40</v>
       </c>
@@ -4967,7 +4996,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="14" t="s">
         <v>43</v>
       </c>
@@ -5005,7 +5034,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="14" t="s">
         <v>46</v>
       </c>
@@ -5043,7 +5072,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="14" t="s">
         <v>49</v>
       </c>
@@ -5081,7 +5110,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="14" t="s">
         <v>52</v>
       </c>
@@ -5117,7 +5146,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="14" t="s">
         <v>55</v>
       </c>
@@ -5153,7 +5182,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="14" t="s">
         <v>58</v>
       </c>
@@ -5189,7 +5218,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="14" t="s">
         <v>61</v>
       </c>
@@ -5225,7 +5254,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="14" t="s">
         <v>64</v>
       </c>
@@ -5261,7 +5290,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="14" t="s">
         <v>68</v>
       </c>
@@ -5297,7 +5326,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="14" t="s">
         <v>72</v>
       </c>
@@ -5333,7 +5362,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="14" t="s">
         <v>76</v>
       </c>
@@ -5369,7 +5398,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="14" t="s">
         <v>80</v>
       </c>
@@ -5405,7 +5434,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="14" t="s">
         <v>84</v>
       </c>
@@ -5441,7 +5470,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="14" t="s">
         <v>87</v>
       </c>
@@ -5477,7 +5506,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="14" t="s">
         <v>90</v>
       </c>
@@ -5513,7 +5542,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" s="14" t="s">
         <v>93</v>
       </c>
@@ -5549,7 +5578,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" s="14" t="s">
         <v>96</v>
       </c>
@@ -5587,7 +5616,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="14" t="s">
         <v>99</v>
       </c>
@@ -5625,7 +5654,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" s="14" t="s">
         <v>102</v>
       </c>
@@ -5663,7 +5692,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" s="14" t="s">
         <v>105</v>
       </c>
@@ -5701,7 +5730,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" s="14" t="s">
         <v>108</v>
       </c>
@@ -5739,7 +5768,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" s="14" t="s">
         <v>111</v>
       </c>
@@ -5777,7 +5806,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" s="14" t="s">
         <v>114</v>
       </c>
@@ -5824,25 +5853,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="44.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="46.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
         <v>246</v>
       </c>
@@ -5880,7 +5909,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
         <v>0</v>
       </c>
@@ -5918,7 +5947,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
         <v>117</v>
       </c>
@@ -5956,7 +5985,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
         <v>1</v>
       </c>
@@ -5994,7 +6023,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>4</v>
       </c>
@@ -6032,7 +6061,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
         <v>7</v>
       </c>
@@ -6070,7 +6099,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
         <v>10</v>
       </c>
@@ -6108,7 +6137,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
         <v>13</v>
       </c>
@@ -6146,7 +6175,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
         <v>16</v>
       </c>
@@ -6184,7 +6213,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
         <v>19</v>
       </c>
@@ -6222,7 +6251,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
         <v>22</v>
       </c>
@@ -6260,7 +6289,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
         <v>25</v>
       </c>
@@ -6298,7 +6327,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="14" t="s">
         <v>28</v>
       </c>
@@ -6336,7 +6365,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="14" t="s">
         <v>31</v>
       </c>
@@ -6374,7 +6403,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>294</v>
       </c>
@@ -6412,7 +6441,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="14" t="s">
         <v>37</v>
       </c>
@@ -6450,7 +6479,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="14" t="s">
         <v>40</v>
       </c>
@@ -6488,7 +6517,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="14" t="s">
         <v>43</v>
       </c>
@@ -6526,7 +6555,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="14" t="s">
         <v>46</v>
       </c>
@@ -6564,7 +6593,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="14" t="s">
         <v>49</v>
       </c>
@@ -6602,7 +6631,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="14" t="s">
         <v>52</v>
       </c>
@@ -6640,7 +6669,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="14" t="s">
         <v>55</v>
       </c>
@@ -6678,7 +6707,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="14" t="s">
         <v>58</v>
       </c>
@@ -6716,7 +6745,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="14" t="s">
         <v>61</v>
       </c>
@@ -6754,7 +6783,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="14" t="s">
         <v>64</v>
       </c>
@@ -6792,7 +6821,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="14" t="s">
         <v>68</v>
       </c>
@@ -6830,7 +6859,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="14" t="s">
         <v>72</v>
       </c>
@@ -6868,7 +6897,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="14" t="s">
         <v>76</v>
       </c>
@@ -6906,7 +6935,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="14" t="s">
         <v>80</v>
       </c>
@@ -6944,7 +6973,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="14" t="s">
         <v>84</v>
       </c>
@@ -6982,7 +7011,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="14" t="s">
         <v>87</v>
       </c>
@@ -7020,7 +7049,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="14" t="s">
         <v>90</v>
       </c>
@@ -7058,7 +7087,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" s="14" t="s">
         <v>93</v>
       </c>
@@ -7096,7 +7125,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" s="14" t="s">
         <v>96</v>
       </c>
@@ -7134,7 +7163,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="14" t="s">
         <v>99</v>
       </c>
@@ -7172,7 +7201,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" s="14" t="s">
         <v>102</v>
       </c>
@@ -7210,7 +7239,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" s="14" t="s">
         <v>105</v>
       </c>
@@ -7248,7 +7277,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" s="14" t="s">
         <v>108</v>
       </c>
@@ -7286,7 +7315,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" s="14" t="s">
         <v>111</v>
       </c>
@@ -7324,7 +7353,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" s="14" t="s">
         <v>114</v>
       </c>
@@ -7373,23 +7402,23 @@
   <sheetViews>
     <sheetView topLeftCell="A33" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="44.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="46.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
         <v>246</v>
       </c>
@@ -7427,7 +7456,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
         <v>0</v>
       </c>
@@ -7463,7 +7492,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
         <v>117</v>
       </c>
@@ -7499,7 +7528,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
         <v>1</v>
       </c>
@@ -7535,7 +7564,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>4</v>
       </c>
@@ -7567,7 +7596,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
         <v>7</v>
       </c>
@@ -7603,7 +7632,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
         <v>10</v>
       </c>
@@ -7639,7 +7668,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
         <v>13</v>
       </c>
@@ -7675,7 +7704,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
         <v>16</v>
       </c>
@@ -7711,7 +7740,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
         <v>19</v>
       </c>
@@ -7747,7 +7776,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
         <v>22</v>
       </c>
@@ -7783,7 +7812,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
         <v>25</v>
       </c>
@@ -7819,7 +7848,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="14" t="s">
         <v>28</v>
       </c>
@@ -7855,7 +7884,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="14" t="s">
         <v>31</v>
       </c>
@@ -7891,7 +7920,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>294</v>
       </c>
@@ -7927,7 +7956,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="14" t="s">
         <v>37</v>
       </c>
@@ -7963,7 +7992,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="14" t="s">
         <v>40</v>
       </c>
@@ -7999,7 +8028,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="14" t="s">
         <v>43</v>
       </c>
@@ -8035,7 +8064,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="14" t="s">
         <v>46</v>
       </c>
@@ -8071,7 +8100,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="14" t="s">
         <v>49</v>
       </c>
@@ -8107,7 +8136,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="14" t="s">
         <v>52</v>
       </c>
@@ -8141,7 +8170,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="14" t="s">
         <v>55</v>
       </c>
@@ -8175,7 +8204,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="14" t="s">
         <v>58</v>
       </c>
@@ -8209,7 +8238,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="14" t="s">
         <v>61</v>
       </c>
@@ -8243,7 +8272,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="14" t="s">
         <v>64</v>
       </c>
@@ -8277,7 +8306,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="14" t="s">
         <v>68</v>
       </c>
@@ -8311,7 +8340,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="14" t="s">
         <v>72</v>
       </c>
@@ -8345,7 +8374,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="14" t="s">
         <v>76</v>
       </c>
@@ -8381,7 +8410,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="14" t="s">
         <v>80</v>
       </c>
@@ -8417,7 +8446,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="14" t="s">
         <v>84</v>
       </c>
@@ -8451,7 +8480,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="14" t="s">
         <v>87</v>
       </c>
@@ -8485,7 +8514,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="14" t="s">
         <v>90</v>
       </c>
@@ -8519,7 +8548,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" s="14" t="s">
         <v>93</v>
       </c>
@@ -8553,7 +8582,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" s="14" t="s">
         <v>96</v>
       </c>
@@ -8589,7 +8618,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="14" t="s">
         <v>99</v>
       </c>
@@ -8625,7 +8654,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" s="14" t="s">
         <v>102</v>
       </c>
@@ -8661,7 +8690,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" s="14" t="s">
         <v>105</v>
       </c>
@@ -8691,7 +8720,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" s="14" t="s">
         <v>108</v>
       </c>
@@ -8721,7 +8750,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" s="14" t="s">
         <v>111</v>
       </c>
@@ -8751,7 +8780,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" s="14" t="s">
         <v>114</v>
       </c>
@@ -8794,23 +8823,23 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="44.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="46.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
         <v>246</v>
       </c>
@@ -8848,7 +8877,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
         <v>0</v>
       </c>
@@ -8876,7 +8905,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
         <v>117</v>
       </c>
@@ -8904,7 +8933,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
         <v>1</v>
       </c>
@@ -8932,7 +8961,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>4</v>
       </c>
@@ -8960,7 +8989,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
         <v>7</v>
       </c>
@@ -8996,7 +9025,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
         <v>10</v>
       </c>
@@ -9024,7 +9053,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
         <v>13</v>
       </c>
@@ -9052,7 +9081,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
         <v>16</v>
       </c>
@@ -9080,7 +9109,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
         <v>19</v>
       </c>
@@ -9108,7 +9137,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
         <v>22</v>
       </c>
@@ -9136,7 +9165,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
         <v>25</v>
       </c>
@@ -9172,7 +9201,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="14" t="s">
         <v>28</v>
       </c>
@@ -9200,7 +9229,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="14" t="s">
         <v>31</v>
       </c>
@@ -9236,7 +9265,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>294</v>
       </c>
@@ -9264,7 +9293,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="14" t="s">
         <v>37</v>
       </c>
@@ -9292,7 +9321,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="14" t="s">
         <v>40</v>
       </c>
@@ -9328,7 +9357,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="14" t="s">
         <v>43</v>
       </c>
@@ -9356,7 +9385,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="14" t="s">
         <v>46</v>
       </c>
@@ -9384,7 +9413,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="14" t="s">
         <v>49</v>
       </c>
@@ -9412,7 +9441,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="14" t="s">
         <v>52</v>
       </c>
@@ -9440,7 +9469,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="14" t="s">
         <v>55</v>
       </c>
@@ -9468,7 +9497,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="14" t="s">
         <v>58</v>
       </c>
@@ -9496,7 +9525,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="14" t="s">
         <v>61</v>
       </c>
@@ -9524,7 +9553,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="14" t="s">
         <v>64</v>
       </c>
@@ -9552,7 +9581,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="14" t="s">
         <v>68</v>
       </c>
@@ -9580,7 +9609,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="14" t="s">
         <v>72</v>
       </c>
@@ -9608,7 +9637,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="14" t="s">
         <v>76</v>
       </c>
@@ -9636,7 +9665,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="14" t="s">
         <v>80</v>
       </c>
@@ -9664,7 +9693,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="14" t="s">
         <v>84</v>
       </c>
@@ -9692,7 +9721,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="14" t="s">
         <v>87</v>
       </c>
@@ -9720,7 +9749,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="14" t="s">
         <v>90</v>
       </c>
@@ -9748,7 +9777,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" s="14" t="s">
         <v>93</v>
       </c>
@@ -9776,7 +9805,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" s="14" t="s">
         <v>96</v>
       </c>
@@ -9804,7 +9833,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="14" t="s">
         <v>99</v>
       </c>
@@ -9832,7 +9861,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" s="14" t="s">
         <v>102</v>
       </c>
@@ -9860,7 +9889,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" s="14" t="s">
         <v>105</v>
       </c>
@@ -9888,7 +9917,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" s="14" t="s">
         <v>108</v>
       </c>
@@ -9916,7 +9945,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" s="14" t="s">
         <v>111</v>
       </c>
@@ -9944,7 +9973,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" s="14" t="s">
         <v>114</v>
       </c>
@@ -9985,17 +10014,17 @@
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="47.44140625" customWidth="1"/>
-    <col min="2" max="2" width="30.88671875" customWidth="1"/>
+    <col min="1" max="1" width="47.5" customWidth="1"/>
+    <col min="2" max="2" width="30.83203125" customWidth="1"/>
     <col min="9" max="9" width="5" customWidth="1"/>
-    <col min="10" max="10" width="25.5546875" customWidth="1"/>
+    <col min="10" max="10" width="25.5" customWidth="1"/>
     <col min="11" max="11" width="25" customWidth="1"/>
-    <col min="12" max="12" width="19.5546875" customWidth="1"/>
+    <col min="12" max="12" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
         <v>246</v>
       </c>
@@ -10033,7 +10062,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
         <v>0</v>
       </c>
@@ -10061,7 +10090,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
         <v>117</v>
       </c>
@@ -10089,7 +10118,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
         <v>1</v>
       </c>
@@ -10117,7 +10146,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>4</v>
       </c>
@@ -10145,7 +10174,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
         <v>7</v>
       </c>
@@ -10177,7 +10206,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
         <v>10</v>
       </c>
@@ -10209,7 +10238,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
         <v>13</v>
       </c>
@@ -10237,7 +10266,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
         <v>16</v>
       </c>
@@ -10265,7 +10294,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
         <v>19</v>
       </c>
@@ -10293,7 +10322,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
         <v>22</v>
       </c>
@@ -10321,7 +10350,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
         <v>25</v>
       </c>
@@ -10353,7 +10382,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="14" t="s">
         <v>28</v>
       </c>
@@ -10381,7 +10410,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="14" t="s">
         <v>31</v>
       </c>
@@ -10413,7 +10442,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>294</v>
       </c>
@@ -10441,7 +10470,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="14" t="s">
         <v>37</v>
       </c>
@@ -10469,7 +10498,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="14" t="s">
         <v>40</v>
       </c>
@@ -10503,7 +10532,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="14" t="s">
         <v>43</v>
       </c>
@@ -10531,7 +10560,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="14" t="s">
         <v>46</v>
       </c>
@@ -10559,7 +10588,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="14" t="s">
         <v>49</v>
       </c>
@@ -10587,7 +10616,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="14" t="s">
         <v>52</v>
       </c>
@@ -10615,7 +10644,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="14" t="s">
         <v>55</v>
       </c>
@@ -10643,7 +10672,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="14" t="s">
         <v>58</v>
       </c>
@@ -10671,7 +10700,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="14" t="s">
         <v>61</v>
       </c>
@@ -10699,7 +10728,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="14" t="s">
         <v>64</v>
       </c>
@@ -10727,7 +10756,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="14" t="s">
         <v>68</v>
       </c>
@@ -10755,7 +10784,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="14" t="s">
         <v>72</v>
       </c>
@@ -10783,7 +10812,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="14" t="s">
         <v>76</v>
       </c>
@@ -10811,7 +10840,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="14" t="s">
         <v>80</v>
       </c>
@@ -10839,7 +10868,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="14" t="s">
         <v>84</v>
       </c>
@@ -10867,7 +10896,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="14" t="s">
         <v>87</v>
       </c>
@@ -10895,7 +10924,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="14" t="s">
         <v>90</v>
       </c>
@@ -10923,7 +10952,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" s="14" t="s">
         <v>93</v>
       </c>
@@ -10951,7 +10980,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" s="14" t="s">
         <v>96</v>
       </c>
@@ -10983,7 +11012,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="14" t="s">
         <v>99</v>
       </c>
@@ -11015,7 +11044,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" s="14" t="s">
         <v>102</v>
       </c>
@@ -11043,7 +11072,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" s="14" t="s">
         <v>105</v>
       </c>
@@ -11071,7 +11100,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" s="14" t="s">
         <v>108</v>
       </c>
@@ -11099,7 +11128,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" s="14" t="s">
         <v>111</v>
       </c>
@@ -11127,7 +11156,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" s="14" t="s">
         <v>114</v>
       </c>
@@ -11155,7 +11184,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" s="14" t="s">
         <v>118</v>
       </c>
@@ -11187,7 +11216,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" s="14" t="s">
         <v>121</v>
       </c>
@@ -11219,7 +11248,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" s="14" t="s">
         <v>428</v>
       </c>
@@ -11249,7 +11278,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" s="14" t="s">
         <v>127</v>
       </c>
@@ -11281,7 +11310,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" s="14" t="s">
         <v>130</v>
       </c>
@@ -11313,7 +11342,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" s="14" t="s">
         <v>133</v>
       </c>
@@ -11345,7 +11374,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" s="14" t="s">
         <v>439</v>
       </c>
@@ -11377,7 +11406,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" s="14" t="s">
         <v>442</v>
       </c>
@@ -11409,7 +11438,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A49" s="14" t="s">
         <v>445</v>
       </c>
@@ -11441,7 +11470,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50" s="14" t="s">
         <v>139</v>
       </c>

</xml_diff>

<commit_message>
add ontology refs to template metadata
</commit_message>
<xml_diff>
--- a/templates/1SPL01_plants.xlsx
+++ b/templates/1SPL01_plants.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dominikbrilhaus/03_DataPLANT_github/SWATE_templates/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EE78103-3C6E-1742-8A3E-115735EF6AA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C02E302-6488-F64B-A160-D640869115F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="-20260" windowWidth="25500" windowHeight="16120" activeTab="1" xr2:uid="{2D1671A6-E5E6-4E90-817E-C23847CD9BD1}"/>
+    <workbookView xWindow="-1120" yWindow="-21100" windowWidth="25560" windowHeight="20280" activeTab="1" xr2:uid="{2D1671A6-E5E6-4E90-817E-C23847CD9BD1}"/>
   </bookViews>
   <sheets>
     <sheet name="1SPL01_plants" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2433" uniqueCount="454">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2441" uniqueCount="459">
   <si>
     <t>Source Name</t>
   </si>
@@ -1431,6 +1431,21 @@
   </si>
   <si>
     <t>[Comment] Author ORCID</t>
+  </si>
+  <si>
+    <t>brilhaus@hhu.de</t>
+  </si>
+  <si>
+    <t>https://orcid.org/0000-0001-9021-3197</t>
+  </si>
+  <si>
+    <t>NFDI4PSO:1000096</t>
+  </si>
+  <si>
+    <t>NFDI4PSO:1000097</t>
+  </si>
+  <si>
+    <t>NFDI4PSO:1000098</t>
   </si>
 </sst>
 </file>
@@ -1605,7 +1620,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1654,6 +1669,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2401,7 +2419,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="629" row="2">
+  <wetp:taskpane dockstate="right" visibility="0" width="350" row="2">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
   <wetp:taskpane dockstate="right" visibility="0" width="662" row="2">
@@ -4015,18 +4033,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C806736B-09AD-44FE-B8F6-60FEE51F74DE}">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="106" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="35.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="57.1640625" customWidth="1"/>
-    <col min="3" max="3" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="57.33203125" customWidth="1"/>
+    <col min="3" max="5" width="18.6640625" customWidth="1"/>
+    <col min="6" max="6" width="45.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -4107,27 +4123,39 @@
         <v>214</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
+      <c r="B10" s="9" t="s">
+        <v>456</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>457</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>458</v>
+      </c>
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
+      <c r="B11" s="9" t="s">
+        <v>265</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>265</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>265</v>
+      </c>
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>452</v>
       </c>
@@ -4135,16 +4163,17 @@
       <c r="C12" s="19"/>
       <c r="D12" s="19"/>
       <c r="E12" s="19"/>
-      <c r="F12" s="9"/>
+      <c r="F12" s="19" t="s">
+        <v>451</v>
+      </c>
     </row>
     <row r="13" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>217</v>
       </c>
       <c r="B13" s="10"/>
-      <c r="F13" s="9"/>
-    </row>
-    <row r="14" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>218</v>
       </c>
@@ -4174,7 +4203,7 @@
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
     </row>
-    <row r="16" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>224</v>
       </c>
@@ -4182,16 +4211,13 @@
       <c r="C16" s="9"/>
       <c r="D16" s="9"/>
       <c r="E16" s="9"/>
-      <c r="F16" s="18" t="s">
-        <v>451</v>
-      </c>
+      <c r="F16" s="9"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
         <v>225</v>
       </c>
       <c r="B17" s="10"/>
-      <c r="F17" s="9"/>
     </row>
     <row r="18" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
@@ -4206,9 +4232,10 @@
       <c r="D18" s="9" t="s">
         <v>229</v>
       </c>
-      <c r="F18" s="9" t="s">
+      <c r="E18" s="9" t="s">
         <v>230</v>
       </c>
+      <c r="F18" s="9"/>
     </row>
     <row r="19" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
@@ -4223,9 +4250,10 @@
       <c r="D19" s="9" t="s">
         <v>234</v>
       </c>
-      <c r="F19" s="9" t="s">
+      <c r="E19" s="9" t="s">
         <v>235</v>
       </c>
+      <c r="F19" s="9"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
@@ -4234,16 +4262,20 @@
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
       <c r="F20" s="9"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
         <v>237</v>
       </c>
       <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="F21" s="9"/>
+      <c r="C21" s="18" t="s">
+        <v>454</v>
+      </c>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
@@ -4252,6 +4284,7 @@
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
       <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
       <c r="F22" s="9"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -4261,6 +4294,7 @@
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
       <c r="F23" s="9"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -4270,6 +4304,7 @@
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
       <c r="F24" s="9"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -4279,23 +4314,26 @@
       <c r="B25" s="9"/>
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
       <c r="F25" s="9"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>453</v>
       </c>
       <c r="B26" s="9"/>
-      <c r="C26" s="19"/>
-      <c r="D26" s="19"/>
-      <c r="F26" s="9"/>
+      <c r="C26" s="20" t="s">
+        <v>455</v>
+      </c>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
         <v>242</v>
       </c>
       <c r="B27" s="10"/>
-      <c r="F27" s="9"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
@@ -4304,6 +4342,7 @@
       <c r="B28" s="11"/>
       <c r="C28" s="9"/>
       <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
       <c r="F28" s="9"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -4313,6 +4352,7 @@
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
       <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
       <c r="F29" s="9"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -4322,15 +4362,18 @@
       <c r="B30" s="12"/>
       <c r="C30" s="9"/>
       <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
       <c r="F30" s="9"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F16" r:id="rId1" display="https://www.ebi.ac.uk/ena/browser/view/ERC000037" xr:uid="{8661B25F-28B7-4001-B986-A010D408E879}"/>
+    <hyperlink ref="F12" r:id="rId1" display="https://www.ebi.ac.uk/ena/browser/view/ERC000037" xr:uid="{8661B25F-28B7-4001-B986-A010D408E879}"/>
+    <hyperlink ref="C21" r:id="rId2" xr:uid="{A67F4947-4B01-9F4B-9C34-7473909B7C41}"/>
+    <hyperlink ref="C26" r:id="rId3" xr:uid="{A94F3EDE-BACC-8E44-BD8B-3C31B67A40AD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <legacyDrawing r:id="rId5"/>
 </worksheet>
 </file>
 

</xml_diff>